<commit_message>
all changes during course
</commit_message>
<xml_diff>
--- a/Lectures/simulated_data.xlsx
+++ b/Lectures/simulated_data.xlsx
@@ -432,16 +432,16 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>4.609094580382852</v>
+        <v>3.835552596714483</v>
       </c>
       <c r="E2">
-        <v>2.809274392406496</v>
+        <v>0.8900544242691064</v>
       </c>
       <c r="F2">
-        <v>104.1855470671699</v>
+        <v>82.51391365710614</v>
       </c>
       <c r="G2">
-        <v>31.08064982394355</v>
+        <v>21.11093335612109</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -455,16 +455,16 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <v>4.504086320992014</v>
+        <v>5.528416835309878</v>
       </c>
       <c r="E3">
-        <v>2.765419122999586</v>
+        <v>0.9086528341696638</v>
       </c>
       <c r="F3">
-        <v>101.6505256846148</v>
+        <v>66.51081684824972</v>
       </c>
       <c r="G3">
-        <v>27.53821724222003</v>
+        <v>32.5356607209018</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -478,16 +478,16 @@
         <v>7</v>
       </c>
       <c r="D4">
-        <v>2.109382966813856</v>
+        <v>3.389014367264778</v>
       </c>
       <c r="E4">
-        <v>2.597593800729837</v>
+        <v>4.125642136441833</v>
       </c>
       <c r="F4">
-        <v>99.96734036225527</v>
+        <v>57.59293919951686</v>
       </c>
       <c r="G4">
-        <v>5.299206261345802</v>
+        <v>4.003238373410056</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -501,16 +501,16 @@
         <v>7</v>
       </c>
       <c r="D5">
-        <v>2.719660187847316</v>
+        <v>1.14708997008554</v>
       </c>
       <c r="E5">
-        <v>2.183409094420599</v>
+        <v>3.076693961165187</v>
       </c>
       <c r="F5">
-        <v>73.77988013095548</v>
+        <v>32.82583326047829</v>
       </c>
       <c r="G5">
-        <v>63.97744134166985</v>
+        <v>82.70594722083857</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -518,22 +518,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6">
-        <v>2.795647562991133</v>
+        <v>5.472265686199302</v>
       </c>
       <c r="E6">
-        <v>3.679280085840327</v>
+        <v>2.66442582073238</v>
       </c>
       <c r="F6">
-        <v>71.29988762208386</v>
+        <v>46.90064166430977</v>
       </c>
       <c r="G6">
-        <v>32.75714077889211</v>
+        <v>27.85683433058443</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -547,16 +547,16 @@
         <v>7</v>
       </c>
       <c r="D7">
-        <v>2.085244206148905</v>
+        <v>1.334743394907734</v>
       </c>
       <c r="E7">
-        <v>2.481648103653793</v>
+        <v>3.896740308473223</v>
       </c>
       <c r="F7">
-        <v>73.63902807181657</v>
+        <v>90.00417312256316</v>
       </c>
       <c r="G7">
-        <v>34.42207399195229</v>
+        <v>33.85122998272168</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -567,19 +567,19 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8">
-        <v>4.056697000061961</v>
+        <v>5.60706370553178</v>
       </c>
       <c r="E8">
-        <v>3.53914979430953</v>
+        <v>3.981403706453577</v>
       </c>
       <c r="F8">
-        <v>80.14069928579825</v>
+        <v>69.17012194640326</v>
       </c>
       <c r="G8">
-        <v>47.15560611502652</v>
+        <v>44.32275577968915</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -593,16 +593,16 @@
         <v>6</v>
       </c>
       <c r="D9">
-        <v>4.629863447541088</v>
+        <v>2.658308209248342</v>
       </c>
       <c r="E9">
-        <v>4.668476957929466</v>
+        <v>4.869141274352523</v>
       </c>
       <c r="F9">
-        <v>37.86512853724089</v>
+        <v>109.0599159400299</v>
       </c>
       <c r="G9">
-        <v>55.64383641886724</v>
+        <v>44.79017057808762</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -616,16 +616,16 @@
         <v>7</v>
       </c>
       <c r="D10">
-        <v>3.648044223839662</v>
+        <v>3.791839669140422</v>
       </c>
       <c r="E10">
-        <v>0.64602051457208</v>
+        <v>3.198720736692172</v>
       </c>
       <c r="F10">
-        <v>76.92044871323245</v>
+        <v>59.55194981035638</v>
       </c>
       <c r="G10">
-        <v>43.95195849742392</v>
+        <v>17.85302097753112</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -633,22 +633,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="D11">
-        <v>4.332654044372989</v>
+        <v>4.568662008538956</v>
       </c>
       <c r="E11">
-        <v>2.47473194935431</v>
+        <v>2.512084667368572</v>
       </c>
       <c r="F11">
-        <v>79.35131724232957</v>
+        <v>97.52252416630938</v>
       </c>
       <c r="G11">
-        <v>64.17640910443497</v>
+        <v>15.09202414934451</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -656,22 +656,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
       </c>
       <c r="D12">
-        <v>5.188582417114884</v>
+        <v>3.884035779029048</v>
       </c>
       <c r="E12">
-        <v>2.596194118657488</v>
+        <v>1.786269840004332</v>
       </c>
       <c r="F12">
-        <v>67.70004525065211</v>
+        <v>67.80077229457494</v>
       </c>
       <c r="G12">
-        <v>36.3966641284779</v>
+        <v>29.98694873542614</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -682,19 +682,19 @@
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D13">
-        <v>3.176391160498981</v>
+        <v>3.169734189657093</v>
       </c>
       <c r="E13">
-        <v>1.865172341706751</v>
+        <v>1.252430595416194</v>
       </c>
       <c r="F13">
-        <v>83.75756113131523</v>
+        <v>57.48898754577474</v>
       </c>
       <c r="G13">
-        <v>18.1089487480661</v>
+        <v>38.87121130161695</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -702,22 +702,22 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D14">
-        <v>3.782114300470206</v>
+        <v>2.654888525402939</v>
       </c>
       <c r="E14">
-        <v>3.944941919353234</v>
+        <v>2.595486170518498</v>
       </c>
       <c r="F14">
-        <v>80.54114722466248</v>
+        <v>111.0655183697489</v>
       </c>
       <c r="G14">
-        <v>38.34815403109477</v>
+        <v>17.25448013471419</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -725,22 +725,22 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="D15">
-        <v>1.188171697206746</v>
+        <v>4.987705425647089</v>
       </c>
       <c r="E15">
-        <v>1.166894999938418</v>
+        <v>3.01075022968644</v>
       </c>
       <c r="F15">
-        <v>89.69027848936069</v>
+        <v>78.40780586747414</v>
       </c>
       <c r="G15">
-        <v>68.12039383235376</v>
+        <v>9.622918861120127</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -748,22 +748,22 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="D16">
-        <v>4.520627157093439</v>
+        <v>4.040161468576324</v>
       </c>
       <c r="E16">
-        <v>1.188933345873618</v>
+        <v>3.177873423813282</v>
       </c>
       <c r="F16">
-        <v>89.13473942787881</v>
+        <v>47.50370270280273</v>
       </c>
       <c r="G16">
-        <v>28.59506695838715</v>
+        <v>23.25523237579559</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -771,22 +771,22 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D17">
-        <v>3.129164076839693</v>
+        <v>4.611214123034634</v>
       </c>
       <c r="E17">
-        <v>2.535339555110719</v>
+        <v>1.880188157187829</v>
       </c>
       <c r="F17">
-        <v>82.71014253673697</v>
+        <v>14.15151714614174</v>
       </c>
       <c r="G17">
-        <v>59.36253260706529</v>
+        <v>60.97035371558065</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -797,19 +797,19 @@
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D18">
-        <v>5.058982372434379</v>
+        <v>5.202128301578574</v>
       </c>
       <c r="E18">
-        <v>2.871720905621635</v>
+        <v>1.708370936279019</v>
       </c>
       <c r="F18">
-        <v>66.35241640443779</v>
+        <v>79.49208813250146</v>
       </c>
       <c r="G18">
-        <v>87.5330195585783</v>
+        <v>24.4913039108656</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -817,22 +817,22 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19">
-        <v>3.362075617837708</v>
+        <v>2.40317936485656</v>
       </c>
       <c r="E19">
-        <v>3.760540814379491</v>
+        <v>3.028417202288276</v>
       </c>
       <c r="F19">
-        <v>18.16295207629087</v>
+        <v>67.95614306222794</v>
       </c>
       <c r="G19">
-        <v>51.43444635604845</v>
+        <v>49.12876283386283</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -840,22 +840,22 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
       </c>
       <c r="D20">
-        <v>2.375819297477618</v>
+        <v>5.773410114174354</v>
       </c>
       <c r="E20">
-        <v>1.212385548639517</v>
+        <v>1.145593332901836</v>
       </c>
       <c r="F20">
-        <v>81.43718228171691</v>
+        <v>30.92956563070015</v>
       </c>
       <c r="G20">
-        <v>39.38545851515138</v>
+        <v>52.32717916647265</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -863,22 +863,22 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D21">
-        <v>5.493280107698358</v>
+        <v>2.483300150669507</v>
       </c>
       <c r="E21">
-        <v>4.035729268650948</v>
+        <v>3.119946118303702</v>
       </c>
       <c r="F21">
-        <v>74.2216240486879</v>
+        <v>73.03745716877749</v>
       </c>
       <c r="G21">
-        <v>41.18989730477023</v>
+        <v>2.36392095913525</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -886,22 +886,22 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
       </c>
       <c r="D22">
-        <v>2.034268618785824</v>
+        <v>4.480341439799051</v>
       </c>
       <c r="E22">
-        <v>2.023169871291196</v>
+        <v>2.776247428601131</v>
       </c>
       <c r="F22">
-        <v>92.43649114361386</v>
+        <v>53.68394077873329</v>
       </c>
       <c r="G22">
-        <v>18.82013309224786</v>
+        <v>8.266991960643239</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -915,16 +915,16 @@
         <v>7</v>
       </c>
       <c r="D23">
-        <v>5.793393697751005</v>
+        <v>2.855144047978813</v>
       </c>
       <c r="E23">
-        <v>4.927255728426049</v>
+        <v>4.55541127322908</v>
       </c>
       <c r="F23">
-        <v>96.25108966039353</v>
+        <v>55.54942968569293</v>
       </c>
       <c r="G23">
-        <v>27.18116196117143</v>
+        <v>74.77261233281929</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -932,22 +932,22 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D24">
-        <v>5.000205175434714</v>
+        <v>5.014938407765021</v>
       </c>
       <c r="E24">
-        <v>3.619661682659735</v>
+        <v>1.765903471329896</v>
       </c>
       <c r="F24">
-        <v>109.7650064811792</v>
+        <v>62.92587192860876</v>
       </c>
       <c r="G24">
-        <v>6.711922906952367</v>
+        <v>28.64320358504051</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -961,16 +961,16 @@
         <v>7</v>
       </c>
       <c r="D25">
-        <v>3.625283217993445</v>
+        <v>1.617373290308243</v>
       </c>
       <c r="E25">
-        <v>2.87575464291497</v>
+        <v>3.236835757540429</v>
       </c>
       <c r="F25">
-        <v>73.85078375279255</v>
+        <v>83.74947681738772</v>
       </c>
       <c r="G25">
-        <v>50.462682250325</v>
+        <v>20.37488766179312</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -984,16 +984,16 @@
         <v>7</v>
       </c>
       <c r="D26">
-        <v>1.995289923664466</v>
+        <v>3.279412145024131</v>
       </c>
       <c r="E26">
-        <v>2.560032042259481</v>
+        <v>2.748276710245083</v>
       </c>
       <c r="F26">
-        <v>37.43609320885167</v>
+        <v>103.391944264572</v>
       </c>
       <c r="G26">
-        <v>2.273613776063715</v>
+        <v>37.91628918599088</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1007,16 +1007,16 @@
         <v>7</v>
       </c>
       <c r="D27">
-        <v>5.291350253274823</v>
+        <v>1.268324829799188</v>
       </c>
       <c r="E27">
-        <v>3.690811421638998</v>
+        <v>2.6881677829729</v>
       </c>
       <c r="F27">
-        <v>60.10666444513771</v>
+        <v>96.42459495483435</v>
       </c>
       <c r="G27">
-        <v>58.19294626248271</v>
+        <v>52.28600153926333</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1030,16 +1030,16 @@
         <v>7</v>
       </c>
       <c r="D28">
-        <v>4.250154672020779</v>
+        <v>3.305634670736914</v>
       </c>
       <c r="E28">
-        <v>2.047779905667947</v>
+        <v>2.954636965382352</v>
       </c>
       <c r="F28">
-        <v>73.08784584883097</v>
+        <v>103.8741821951283</v>
       </c>
       <c r="G28">
-        <v>43.86932158241728</v>
+        <v>9.80815823909289</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1047,22 +1047,22 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D29">
-        <v>3.132751820006873</v>
+        <v>4.11943106965656</v>
       </c>
       <c r="E29">
-        <v>3.312075862467313</v>
+        <v>3.222156737950528</v>
       </c>
       <c r="F29">
-        <v>37.05066887030103</v>
+        <v>44.98787656091629</v>
       </c>
       <c r="G29">
-        <v>57.16850734611042</v>
+        <v>51.87109010646878</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1070,22 +1070,22 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C30" t="s">
         <v>7</v>
       </c>
       <c r="D30">
-        <v>4.833266268266597</v>
+        <v>1.46782996063464</v>
       </c>
       <c r="E30">
-        <v>4.067842814467493</v>
+        <v>0.9354427891678414</v>
       </c>
       <c r="F30">
-        <v>108.220443562948</v>
+        <v>102.2973868545321</v>
       </c>
       <c r="G30">
-        <v>46.20584335337828</v>
+        <v>16.99455144233779</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1099,16 +1099,16 @@
         <v>7</v>
       </c>
       <c r="D31">
-        <v>5.728355323050622</v>
+        <v>5.126430890697522</v>
       </c>
       <c r="E31">
-        <v>3.203608416632513</v>
+        <v>2.103556019619417</v>
       </c>
       <c r="F31">
-        <v>61.0501777289395</v>
+        <v>30.01080678860274</v>
       </c>
       <c r="G31">
-        <v>18.53115299175039</v>
+        <v>8.278917356527998</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1116,22 +1116,22 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C32" t="s">
         <v>7</v>
       </c>
       <c r="D32">
-        <v>5.432974256748969</v>
+        <v>5.542401837991629</v>
       </c>
       <c r="E32">
-        <v>4.223713646851518</v>
+        <v>1.770578489139599</v>
       </c>
       <c r="F32">
-        <v>104.169970262896</v>
+        <v>53.46239368871557</v>
       </c>
       <c r="G32">
-        <v>26.86350820853765</v>
+        <v>25.64062600802293</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1145,16 +1145,16 @@
         <v>6</v>
       </c>
       <c r="D33">
-        <v>0.6107279803142469</v>
+        <v>4.578020577209354</v>
       </c>
       <c r="E33">
-        <v>3.491988255470572</v>
+        <v>4.439530085552135</v>
       </c>
       <c r="F33">
-        <v>76.34601912855388</v>
+        <v>105.330048551436</v>
       </c>
       <c r="G33">
-        <v>26.02052589931051</v>
+        <v>7.25977202303514</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1162,22 +1162,22 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D34">
-        <v>5.675535981405733</v>
+        <v>5.536154577008677</v>
       </c>
       <c r="E34">
-        <v>4.357142834226794</v>
+        <v>4.460778253903222</v>
       </c>
       <c r="F34">
-        <v>56.78285968077172</v>
+        <v>46.94265933512254</v>
       </c>
       <c r="G34">
-        <v>6.83134212260407</v>
+        <v>24.98682831039027</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1191,16 +1191,16 @@
         <v>7</v>
       </c>
       <c r="D35">
-        <v>3.014853697360556</v>
+        <v>4.070029369956201</v>
       </c>
       <c r="E35">
-        <v>2.980973701534849</v>
+        <v>1.314548332149332</v>
       </c>
       <c r="F35">
-        <v>87.29224834027239</v>
+        <v>99.98400643029271</v>
       </c>
       <c r="G35">
-        <v>29.37733667875381</v>
+        <v>24.78546260633074</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1208,22 +1208,22 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
       </c>
       <c r="D36">
-        <v>3.495622948929895</v>
+        <v>4.13050602351068</v>
       </c>
       <c r="E36">
-        <v>0.7951915185078609</v>
+        <v>1.84923289102613</v>
       </c>
       <c r="F36">
-        <v>56.74072478301059</v>
+        <v>38.18881980785324</v>
       </c>
       <c r="G36">
-        <v>7.225426872678426</v>
+        <v>49.52627060765283</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1237,16 +1237,16 @@
         <v>7</v>
       </c>
       <c r="D37">
-        <v>3.914552928262602</v>
+        <v>3.740069442241901</v>
       </c>
       <c r="E37">
-        <v>3.160608031778781</v>
+        <v>4.965834576475836</v>
       </c>
       <c r="F37">
-        <v>92.89507099392539</v>
+        <v>69.75672752698343</v>
       </c>
       <c r="G37">
-        <v>19.06862566320545</v>
+        <v>22.90176399753538</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1254,22 +1254,22 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D38">
-        <v>3.398616667141657</v>
+        <v>2.024905419713451</v>
       </c>
       <c r="E38">
-        <v>3.797284409875165</v>
+        <v>2.748428536197414</v>
       </c>
       <c r="F38">
-        <v>101.1583622238647</v>
+        <v>107.8947483022908</v>
       </c>
       <c r="G38">
-        <v>14.72141543044991</v>
+        <v>60.36424653746716</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1283,16 +1283,16 @@
         <v>7</v>
       </c>
       <c r="D39">
-        <v>3.942233086706096</v>
+        <v>3.364224436196156</v>
       </c>
       <c r="E39">
-        <v>4.924657033569105</v>
+        <v>3.63289453373013</v>
       </c>
       <c r="F39">
-        <v>66.38193192902571</v>
+        <v>109.0292371839198</v>
       </c>
       <c r="G39">
-        <v>3.365772813017345</v>
+        <v>9.655572632712392</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1303,19 +1303,19 @@
         <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D40">
-        <v>3.714399884549643</v>
+        <v>1.00427808175715</v>
       </c>
       <c r="E40">
-        <v>2.404415195932411</v>
+        <v>4.231066838955764</v>
       </c>
       <c r="F40">
-        <v>77.92351363535759</v>
+        <v>27.10662553974002</v>
       </c>
       <c r="G40">
-        <v>64.93414152454798</v>
+        <v>48.11671031583285</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1329,16 +1329,16 @@
         <v>7</v>
       </c>
       <c r="D41">
-        <v>5.147492647569331</v>
+        <v>2.327331747953587</v>
       </c>
       <c r="E41">
-        <v>4.559183187817454</v>
+        <v>1.649648301856178</v>
       </c>
       <c r="F41">
-        <v>80.81942347659559</v>
+        <v>83.02666032307613</v>
       </c>
       <c r="G41">
-        <v>60.45068351093096</v>
+        <v>80.09307901952238</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1352,16 +1352,16 @@
         <v>7</v>
       </c>
       <c r="D42">
-        <v>4.621367018861604</v>
+        <v>3.586362490593167</v>
       </c>
       <c r="E42">
-        <v>5.660371464288619</v>
+        <v>2.011741632832168</v>
       </c>
       <c r="F42">
-        <v>109.2718965834486</v>
+        <v>40.23731518777672</v>
       </c>
       <c r="G42">
-        <v>4.591243181806988</v>
+        <v>31.48549259107155</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1372,19 +1372,19 @@
         <v>6</v>
       </c>
       <c r="C43" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D43">
-        <v>3.847336494450283</v>
+        <v>5.324985203761658</v>
       </c>
       <c r="E43">
-        <v>1.084555176150618</v>
+        <v>2.01208558039467</v>
       </c>
       <c r="F43">
-        <v>94.90525946569841</v>
+        <v>91.02972873571527</v>
       </c>
       <c r="G43">
-        <v>10.77719106751357</v>
+        <v>61.48018884849137</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1398,16 +1398,16 @@
         <v>7</v>
       </c>
       <c r="D44">
-        <v>2.57421555474393</v>
+        <v>5.580290780338933</v>
       </c>
       <c r="E44">
-        <v>2.665568399626825</v>
+        <v>2.334300902026008</v>
       </c>
       <c r="F44">
-        <v>66.63921514052306</v>
+        <v>53.20344050102381</v>
       </c>
       <c r="G44">
-        <v>66.63957948563765</v>
+        <v>8.45553074898983</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1421,16 +1421,16 @@
         <v>7</v>
       </c>
       <c r="D45">
-        <v>3.540466232088777</v>
+        <v>2.639975240810683</v>
       </c>
       <c r="E45">
-        <v>3.756774378163282</v>
+        <v>1.851722356976063</v>
       </c>
       <c r="F45">
-        <v>92.73633160365345</v>
+        <v>10.19196290103863</v>
       </c>
       <c r="G45">
-        <v>18.71086368263059</v>
+        <v>79.86685558489862</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1438,22 +1438,22 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C46" t="s">
         <v>7</v>
       </c>
       <c r="D46">
-        <v>1.534222218099357</v>
+        <v>5.083850765877295</v>
       </c>
       <c r="E46">
-        <v>1.823644015646987</v>
+        <v>1.786542026895287</v>
       </c>
       <c r="F46">
-        <v>22.79589919466627</v>
+        <v>70.31000835727554</v>
       </c>
       <c r="G46">
-        <v>26.05927307594425</v>
+        <v>13.07178629525745</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1467,16 +1467,16 @@
         <v>7</v>
       </c>
       <c r="D47">
-        <v>0.7670647977642806</v>
+        <v>2.475473898118651</v>
       </c>
       <c r="E47">
-        <v>2.828257614098322</v>
+        <v>1.823435809622131</v>
       </c>
       <c r="F47">
-        <v>89.54574995673133</v>
+        <v>31.37263717508207</v>
       </c>
       <c r="G47">
-        <v>49.27461093998656</v>
+        <v>46.00664821327582</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1490,16 +1490,16 @@
         <v>7</v>
       </c>
       <c r="D48">
-        <v>1.430751411126358</v>
+        <v>5.112751282838721</v>
       </c>
       <c r="E48">
-        <v>1.238513404306985</v>
+        <v>3.122664933071259</v>
       </c>
       <c r="F48">
-        <v>33.45971901757044</v>
+        <v>77.55997068462763</v>
       </c>
       <c r="G48">
-        <v>38.86594839913816</v>
+        <v>25.90278980941395</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1513,16 +1513,16 @@
         <v>7</v>
       </c>
       <c r="D49">
-        <v>5.565087917334656</v>
+        <v>5.043204928325432</v>
       </c>
       <c r="E49">
-        <v>2.336391207064877</v>
+        <v>1.508193845843718</v>
       </c>
       <c r="F49">
-        <v>63.16732101188038</v>
+        <v>98.79771630100844</v>
       </c>
       <c r="G49">
-        <v>28.97026565178925</v>
+        <v>3.689468971030637</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1533,19 +1533,19 @@
         <v>6</v>
       </c>
       <c r="C50" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D50">
-        <v>1.747979750024893</v>
+        <v>3.242160495395595</v>
       </c>
       <c r="E50">
-        <v>2.8584887390172</v>
+        <v>3.425095578988311</v>
       </c>
       <c r="F50">
-        <v>75.7091069503758</v>
+        <v>52.27609269247633</v>
       </c>
       <c r="G50">
-        <v>9.475456461786194</v>
+        <v>31.07932218109558</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1553,22 +1553,22 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D51">
-        <v>4.844704650497857</v>
+        <v>3.582010385333696</v>
       </c>
       <c r="E51">
-        <v>4.117100511610056</v>
+        <v>2.633178368107929</v>
       </c>
       <c r="F51">
-        <v>28.88328684555109</v>
+        <v>88.51801641846555</v>
       </c>
       <c r="G51">
-        <v>5.06284954928158</v>
+        <v>37.75881390453094</v>
       </c>
     </row>
   </sheetData>

</xml_diff>